<commit_message>
add a attribute that shows supply from each scale
</commit_message>
<xml_diff>
--- a/user_input_data/input_uni.xlsx
+++ b/user_input_data/input_uni.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">State</t>
   </si>
   <si>
-    <t xml:space="preserve">Ohio</t>
+    <t xml:space="preserve">Wisconsin</t>
   </si>
   <si>
     <t xml:space="preserve">Geo-unit process</t>
@@ -187,7 +187,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>